<commit_message>
Fix for SOFP comments
</commit_message>
<xml_diff>
--- a/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.39.xlsx
+++ b/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.39.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\afs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32561FE7-BDCB-4332-BF6A-CCF300EFC1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E02186-B84A-49DD-9EBC-ABDDFF69DABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1710" windowWidth="17925" windowHeight="13110" tabRatio="601" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="1" r:id="rId1"/>
@@ -11044,8 +11044,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:XEW18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13183,7 +13183,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15088,12 +15088,12 @@
   </sheetPr>
   <dimension ref="A1:AH631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="F137" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B6" sqref="B6"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I146" sqref="I146"/>
+      <selection pane="bottomRight" activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -47842,8 +47842,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:XFB64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48516,10 +48516,7 @@
         <f>Data!I152</f>
         <v>44418</v>
       </c>
-      <c r="C59" s="119">
-        <f>B59</f>
-        <v>44418</v>
-      </c>
+      <c r="C59" s="119"/>
       <c r="D59" s="96"/>
     </row>
     <row r="60" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>